<commit_message>
Correcion para validar si un credito es aprobado o rechazado
Signed-off-by: MIGUEL <miguel@miguel-Satellite-L635.(none)>
</commit_message>
<xml_diff>
--- a/docs/template.xlsx
+++ b/docs/template.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="21680" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="114210" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -79,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,17 +405,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -444,13 +440,13 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>B5*2</f>
         <v>0</v>
       </c>
@@ -459,18 +455,14 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="b">
-        <f>A5 &gt; C5</f>
+      <c r="B7" s="1">
+        <f>A5-C5</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>